<commit_message>
test case2 5 dof ddqn
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/xlsx/tested_state_original_design_case2.xlsx
+++ b/dynamics/src/dynamics/xlsx/tested_state_original_design_case2.xlsx
@@ -446,10 +446,10 @@
         <v>23.964</v>
       </c>
       <c r="H1" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="I1" t="n">
-        <v>25.1</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="2">
@@ -477,10 +477,10 @@
         <v>23.964</v>
       </c>
       <c r="H2" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="I2" t="n">
-        <v>25.1</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="3">
@@ -508,10 +508,10 @@
         <v>23.964</v>
       </c>
       <c r="H3" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="I3" t="n">
-        <v>25.1</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="4">
@@ -539,10 +539,10 @@
         <v>23.964</v>
       </c>
       <c r="H4" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="I4" t="n">
-        <v>25.1</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="5">
@@ -570,10 +570,10 @@
         <v>23.964</v>
       </c>
       <c r="H5" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="I5" t="n">
-        <v>25.1</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="6">
@@ -601,10 +601,10 @@
         <v>23.964</v>
       </c>
       <c r="H6" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="I6" t="n">
-        <v>25.1</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="7">
@@ -632,10 +632,10 @@
         <v>23.964</v>
       </c>
       <c r="H7" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="I7" t="n">
-        <v>25.1</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="8">
@@ -663,10 +663,10 @@
         <v>23.964</v>
       </c>
       <c r="H8" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="I8" t="n">
-        <v>25.1</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="9">
@@ -694,10 +694,10 @@
         <v>23.964</v>
       </c>
       <c r="H9" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="I9" t="n">
-        <v>25.1</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="10">
@@ -725,10 +725,10 @@
         <v>23.964</v>
       </c>
       <c r="H10" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="I10" t="n">
-        <v>25.1</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="11">
@@ -756,10 +756,10 @@
         <v>23.964</v>
       </c>
       <c r="H11" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="I11" t="n">
-        <v>25.1</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="12">
@@ -787,10 +787,10 @@
         <v>23.964</v>
       </c>
       <c r="H12" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="I12" t="n">
-        <v>25.1</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="13">
@@ -818,10 +818,10 @@
         <v>23.964</v>
       </c>
       <c r="H13" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="I13" t="n">
-        <v>25.1</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="14">
@@ -849,10 +849,10 @@
         <v>23.964</v>
       </c>
       <c r="H14" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="I14" t="n">
-        <v>25.1</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="15">
@@ -862,7 +862,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" t="n">
         <v>176.3651844588868</v>
@@ -880,10 +880,10 @@
         <v>23.964</v>
       </c>
       <c r="H15" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="I15" t="n">
-        <v>25.1</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="16">
@@ -911,10 +911,10 @@
         <v>23.964</v>
       </c>
       <c r="H16" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="I16" t="n">
-        <v>25.1</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="17">
@@ -942,10 +942,10 @@
         <v>23.964</v>
       </c>
       <c r="H17" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="I17" t="n">
-        <v>25.1</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="18">
@@ -973,10 +973,10 @@
         <v>23.964</v>
       </c>
       <c r="H18" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="I18" t="n">
-        <v>25.1</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="19">
@@ -1004,10 +1004,10 @@
         <v>23.964</v>
       </c>
       <c r="H19" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="I19" t="n">
-        <v>25.1</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="20">
@@ -1035,10 +1035,10 @@
         <v>23.964</v>
       </c>
       <c r="H20" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="I20" t="n">
-        <v>25.1</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="21">
@@ -1048,7 +1048,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C21" t="n">
         <v>328.1082605273225</v>
@@ -1066,10 +1066,10 @@
         <v>23.964</v>
       </c>
       <c r="H21" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="I21" t="n">
-        <v>25.1</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="22">
@@ -1079,7 +1079,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C22" t="n">
         <v>714.3960623361766</v>
@@ -1097,10 +1097,10 @@
         <v>23.964</v>
       </c>
       <c r="H22" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="I22" t="n">
-        <v>25.1</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="23">
@@ -1110,7 +1110,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" t="n">
         <v>252.9776295074435</v>
@@ -1128,10 +1128,10 @@
         <v>23.964</v>
       </c>
       <c r="H23" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="I23" t="n">
-        <v>25.1</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="24">
@@ -1141,7 +1141,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24" t="n">
         <v>710.8878589930479</v>
@@ -1159,10 +1159,10 @@
         <v>23.964</v>
       </c>
       <c r="H24" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="I24" t="n">
-        <v>25.1</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="25">
@@ -1190,10 +1190,10 @@
         <v>23.964</v>
       </c>
       <c r="H25" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="I25" t="n">
-        <v>25.1</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="26">
@@ -1221,10 +1221,10 @@
         <v>23.964</v>
       </c>
       <c r="H26" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="I26" t="n">
-        <v>25.1</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="27">
@@ -1234,7 +1234,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C27" t="n">
         <v>481.9949231290301</v>
@@ -1252,10 +1252,10 @@
         <v>23.964</v>
       </c>
       <c r="H27" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="I27" t="n">
-        <v>25.1</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="28">
@@ -1265,7 +1265,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C28" t="n">
         <v>1053.149130220529</v>
@@ -1283,10 +1283,10 @@
         <v>23.964</v>
       </c>
       <c r="H28" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="I28" t="n">
-        <v>25.1</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="29">
@@ -1314,10 +1314,10 @@
         <v>23.964</v>
       </c>
       <c r="H29" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="I29" t="n">
-        <v>25.1</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="30">
@@ -1327,7 +1327,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C30" t="n">
         <v>1035.728958161156</v>
@@ -1345,10 +1345,10 @@
         <v>23.964</v>
       </c>
       <c r="H30" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="I30" t="n">
-        <v>25.1</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="31">
@@ -1376,10 +1376,10 @@
         <v>23.964</v>
       </c>
       <c r="H31" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="I31" t="n">
-        <v>25.1</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="32">
@@ -1407,10 +1407,10 @@
         <v>23.964</v>
       </c>
       <c r="H32" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="I32" t="n">
-        <v>25.1</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="33">
@@ -1438,10 +1438,10 @@
         <v>23.964</v>
       </c>
       <c r="H33" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="I33" t="n">
-        <v>25.1</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="34">
@@ -1451,7 +1451,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C34" t="n">
         <v>1222.999659563553</v>
@@ -1469,10 +1469,10 @@
         <v>23.964</v>
       </c>
       <c r="H34" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="I34" t="n">
-        <v>25.1</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="35">
@@ -1482,7 +1482,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C35" t="n">
         <v>425.7680034249445</v>
@@ -1500,10 +1500,10 @@
         <v>23.964</v>
       </c>
       <c r="H35" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="I35" t="n">
-        <v>25.1</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="36">
@@ -1513,7 +1513,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C36" t="n">
         <v>1198.298641575391</v>
@@ -1531,10 +1531,10 @@
         <v>23.964</v>
       </c>
       <c r="H36" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="I36" t="n">
-        <v>25.1</v>
+        <v>25.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>